<commit_message>
Getting ready to integrate survey data, made sublist
Got some survey data from rachel, but finalizing sublist with her before I can integrate it into the 'cleaned' data.
</commit_message>
<xml_diff>
--- a/accom_clean.xlsx
+++ b/accom_clean.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tu\cla\Jarcho\STUDIES\Accommodation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tul67061/Documents/GitHub/accomodation/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE66A5C4-7E99-4C4A-829A-A2E211582188}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20970" windowHeight="7380"/>
+    <workbookView xWindow="2280" yWindow="9580" windowWidth="40340" windowHeight="21860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -358,19 +359,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" customWidth="1"/>
+    <col min="14" max="14" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -387,7 +389,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>172</v>
       </c>
@@ -404,7 +406,7 @@
         <v>-15.691700000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>182</v>
       </c>
@@ -421,7 +423,7 @@
         <v>-18.741499999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>208</v>
       </c>
@@ -438,7 +440,7 @@
         <v>-22.1617</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>241</v>
       </c>
@@ -455,7 +457,7 @@
         <v>-23.649899999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>247</v>
       </c>
@@ -472,7 +474,7 @@
         <v>-26.548200000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>273</v>
       </c>
@@ -489,7 +491,7 @@
         <v>-5.6447000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>281</v>
       </c>
@@ -506,7 +508,7 @@
         <v>-12.915900000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>292</v>
       </c>
@@ -523,7 +525,7 @@
         <v>-11.246</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>313</v>
       </c>
@@ -540,7 +542,7 @@
         <v>-5.2820999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>331</v>
       </c>
@@ -557,7 +559,7 @@
         <v>-5.6172000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>333</v>
       </c>
@@ -574,7 +576,7 @@
         <v>-13.2189</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>346</v>
       </c>
@@ -591,7 +593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>369</v>
       </c>
@@ -608,7 +610,7 @@
         <v>-6.2565999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>379</v>
       </c>
@@ -625,7 +627,7 @@
         <v>-14.695</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>386</v>
       </c>
@@ -642,7 +644,7 @@
         <v>-8.6984999999999992</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>422</v>
       </c>
@@ -659,7 +661,7 @@
         <v>-9.4206000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>435</v>
       </c>
@@ -676,7 +678,7 @@
         <v>-7.9787999999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>439</v>
       </c>
@@ -693,7 +695,7 @@
         <v>-4.1764000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>446</v>
       </c>
@@ -710,7 +712,7 @@
         <v>-10.3461</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>454</v>
       </c>
@@ -727,7 +729,7 @@
         <v>-5.2962999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>477</v>
       </c>
@@ -744,7 +746,7 @@
         <v>13.067500000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>481</v>
       </c>
@@ -761,7 +763,7 @@
         <v>-10.6656</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>488</v>
       </c>
@@ -778,7 +780,7 @@
         <v>-12.4946</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>514</v>
       </c>
@@ -795,7 +797,7 @@
         <v>-19.930299999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>555</v>
       </c>
@@ -812,7 +814,7 @@
         <v>-9.9946999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>503</v>
       </c>
@@ -829,7 +831,7 @@
         <v>-7.968</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>523</v>
       </c>
@@ -846,7 +848,7 @@
         <v>-4.5777000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>428</v>
       </c>
@@ -863,7 +865,7 @@
         <v>-13.302199999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>578</v>
       </c>
@@ -880,7 +882,7 @@
         <v>-16.899000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>582</v>
       </c>
@@ -897,7 +899,7 @@
         <v>-12.384499999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>593</v>
       </c>
@@ -914,7 +916,7 @@
         <v>-22.876300000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>420</v>
       </c>
@@ -931,7 +933,7 @@
         <v>-16.586300000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>300</v>
       </c>
@@ -948,7 +950,7 @@
         <v>-7.0784000000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>388</v>
       </c>
@@ -965,7 +967,7 @@
         <v>-12.1021</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>606</v>
       </c>
@@ -982,7 +984,7 @@
         <v>-11.4946</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>525</v>
       </c>
@@ -999,7 +1001,7 @@
         <v>-35.350499999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>571</v>
       </c>
@@ -1016,7 +1018,7 @@
         <v>-10.3619</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>601</v>
       </c>
@@ -1033,7 +1035,7 @@
         <v>-13.5823</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>624</v>
       </c>
@@ -1050,7 +1052,7 @@
         <v>-11.1379</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>542</v>
       </c>
@@ -1067,7 +1069,7 @@
         <v>-12.7334</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>609</v>
       </c>
@@ -1084,7 +1086,7 @@
         <v>-16.610700000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>611</v>
       </c>
@@ -1101,7 +1103,7 @@
         <v>-8.2516999999999996</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>667</v>
       </c>
@@ -1118,7 +1120,7 @@
         <v>-9.2148000000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>161</v>
       </c>
@@ -1135,7 +1137,7 @@
         <v>-17.494</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>584</v>
       </c>
@@ -1152,7 +1154,7 @@
         <v>-7.2195999999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>619</v>
       </c>
@@ -1169,7 +1171,7 @@
         <v>-7.6651999999999996</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>628</v>
       </c>
@@ -1186,7 +1188,7 @@
         <v>-11.4047</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>673</v>
       </c>
@@ -1203,7 +1205,7 @@
         <v>-7.4508000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>696</v>
       </c>
@@ -1220,7 +1222,7 @@
         <v>-12.210100000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>678</v>
       </c>
@@ -1237,7 +1239,7 @@
         <v>-14.5359</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>694</v>
       </c>
@@ -1254,7 +1256,7 @@
         <v>-5.5016999999999996</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>701</v>
       </c>
@@ -1271,7 +1273,7 @@
         <v>-10.0654</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>692</v>
       </c>
@@ -1288,7 +1290,7 @@
         <v>-5.7019000000000002</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>707</v>
       </c>
@@ -1305,7 +1307,7 @@
         <v>-14.531700000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>730</v>
       </c>
@@ -1322,7 +1324,7 @@
         <v>-14.2645</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>308</v>
       </c>
@@ -1339,7 +1341,7 @@
         <v>-1.1324E-14</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>4736</v>
       </c>
@@ -1356,7 +1358,7 @@
         <v>-1.4200000000000001E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>4803</v>
       </c>
@@ -1373,7 +1375,7 @@
         <v>-9.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>4789</v>
       </c>
@@ -1390,7 +1392,7 @@
         <v>-1.54E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>4788</v>
       </c>
@@ -1407,7 +1409,7 @@
         <v>-2.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>4797</v>
       </c>
@@ -1424,7 +1426,7 @@
         <v>-8.8000000000000005E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>589</v>
       </c>
@@ -1441,7 +1443,7 @@
         <v>-1.5432999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>4800</v>
       </c>
@@ -1458,7 +1460,7 @@
         <v>-1.1324E-14</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>453</v>
       </c>

</xml_diff>

<commit_message>
getting ready to add more survey info
</commit_message>
<xml_diff>
--- a/accom_clean.xlsx
+++ b/accom_clean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tul67061/Documents/GitHub/accomodation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE66A5C4-7E99-4C4A-829A-A2E211582188}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4992A5B-911C-A14D-80FF-2EF0080ABD34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="9580" windowWidth="40340" windowHeight="21860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="5860" windowWidth="40340" windowHeight="21860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -369,6 +369,9 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="29.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
     <col min="14" max="14" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
data updated, added exclusion cat. to accom_clean to handle DD analysis
</commit_message>
<xml_diff>
--- a/accom_clean.xlsx
+++ b/accom_clean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tul67061/Documents/GitHub/accomodation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4992A5B-911C-A14D-80FF-2EF0080ABD34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B85F019-37F6-2649-96BB-C44E6CB01A45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="5860" windowWidth="40340" windowHeight="21860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="1080" windowWidth="13440" windowHeight="21860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -363,7 +363,7 @@
   <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updating data for bayes package, next redo analysis
</commit_message>
<xml_diff>
--- a/accom_clean.xlsx
+++ b/accom_clean.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="198">
   <si>
     <t>HouseholdID</t>
   </si>
@@ -673,7 +673,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -688,11 +688,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -719,6 +734,12 @@
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -937,10 +958,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BA68"/>
+  <dimension ref="A1:BM69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="AY52" workbookViewId="0">
+      <selection activeCell="BC83" sqref="BC83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4822,7 +4843,9 @@
       <c r="C25" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D25" s="1"/>
+      <c r="D25" s="1">
+        <v>7.1000000000000002E-4</v>
+      </c>
       <c r="E25">
         <v>7.1000000000000004E-3</v>
       </c>
@@ -5428,7 +5451,9 @@
       <c r="C29" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D29" s="1"/>
+      <c r="D29" s="16">
+        <v>6.3000000000000003E-4</v>
+      </c>
       <c r="E29">
         <v>2.8999999999999998E-3</v>
       </c>
@@ -5587,7 +5612,9 @@
       <c r="C30" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D30" s="1"/>
+      <c r="D30" s="16">
+        <v>7.6999999999999996E-4</v>
+      </c>
       <c r="E30">
         <v>8.8999999999999999E-3</v>
       </c>
@@ -5907,7 +5934,9 @@
       <c r="C32" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D32" s="1"/>
+      <c r="D32" s="16">
+        <v>8.8999999999999995E-4</v>
+      </c>
       <c r="E32">
         <v>1.6999999999999999E-3</v>
       </c>
@@ -6066,7 +6095,9 @@
       <c r="C33" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D33" s="1"/>
+      <c r="D33" s="16">
+        <v>4.8000000000000001E-4</v>
+      </c>
       <c r="E33">
         <v>0.2525</v>
       </c>
@@ -6225,7 +6256,9 @@
       <c r="C34" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D34" s="1"/>
+      <c r="D34" s="16">
+        <v>7.2999999999999996E-4</v>
+      </c>
       <c r="E34">
         <v>2.2800000000000001E-2</v>
       </c>
@@ -6384,7 +6417,9 @@
       <c r="C35" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D35" s="1"/>
+      <c r="D35" s="16">
+        <v>1.4E-3</v>
+      </c>
       <c r="E35">
         <v>2.18E-2</v>
       </c>
@@ -6543,7 +6578,9 @@
       <c r="C36" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D36" s="1"/>
+      <c r="D36" s="16">
+        <v>3.8000000000000002E-4</v>
+      </c>
       <c r="E36">
         <v>3.8999999999999998E-3</v>
       </c>
@@ -6702,7 +6739,9 @@
       <c r="C37" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D37" s="1"/>
+      <c r="D37" s="16">
+        <v>2.3999999999999998E-3</v>
+      </c>
       <c r="E37">
         <v>3.8800000000000001E-2</v>
       </c>
@@ -6861,7 +6900,9 @@
       <c r="C38" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D38" s="1"/>
+      <c r="D38" s="16">
+        <v>4.4999999999999999E-4</v>
+      </c>
       <c r="E38">
         <v>7.3200000000000001E-2</v>
       </c>
@@ -7020,7 +7061,9 @@
       <c r="C39" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D39" s="1"/>
+      <c r="D39" s="16">
+        <v>5.8E-4</v>
+      </c>
       <c r="E39">
         <v>8.6E-3</v>
       </c>
@@ -7179,7 +7222,9 @@
       <c r="C40" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D40" s="1"/>
+      <c r="D40" s="16">
+        <v>4.2000000000000002E-4</v>
+      </c>
       <c r="E40">
         <v>5.5999999999999999E-3</v>
       </c>
@@ -7499,7 +7544,9 @@
       <c r="C42" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D42" s="3"/>
+      <c r="D42" s="16">
+        <v>5.6999999999999998E-4</v>
+      </c>
       <c r="E42">
         <v>0.2525</v>
       </c>
@@ -8139,7 +8186,9 @@
       <c r="C46" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D46" s="3"/>
+      <c r="D46" s="16">
+        <v>7.2999999999999996E-4</v>
+      </c>
       <c r="E46">
         <v>7.7899999999999997E-2</v>
       </c>
@@ -8298,8 +8347,8 @@
       <c r="C47" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="D47" s="3">
-        <v>3.4000000000000002E-4</v>
+      <c r="D47" s="16">
+        <v>6.6E-4</v>
       </c>
       <c r="E47">
         <v>3.9899999999999998E-2</v>
@@ -8942,7 +8991,9 @@
       <c r="C51" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D51" s="3"/>
+      <c r="D51" s="16">
+        <v>5.6999999999999998E-4</v>
+      </c>
       <c r="E51">
         <v>2.4899999999999999E-2</v>
       </c>
@@ -9429,7 +9480,7 @@
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
       <c r="I54" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J54" s="3" t="s">
         <v>53</v>
@@ -9574,7 +9625,9 @@
       <c r="C55" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D55" s="3"/>
+      <c r="D55" s="16">
+        <v>8.5999999999999998E-4</v>
+      </c>
       <c r="E55">
         <v>0.25009999999999999</v>
       </c>
@@ -9733,7 +9786,9 @@
       <c r="C56" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D56" s="3"/>
+      <c r="D56" s="16">
+        <v>4.6000000000000001E-4</v>
+      </c>
       <c r="E56">
         <v>8.6999999999999994E-3</v>
       </c>
@@ -9892,7 +9947,9 @@
       <c r="C57" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D57" s="3"/>
+      <c r="D57" s="16">
+        <v>8.0999999999999996E-4</v>
+      </c>
       <c r="E57">
         <v>0.1371</v>
       </c>
@@ -10051,7 +10108,9 @@
       <c r="C58" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D58" s="3"/>
+      <c r="D58" s="16">
+        <v>2.1000000000000001E-4</v>
+      </c>
       <c r="E58">
         <v>8.8700000000000001E-2</v>
       </c>
@@ -10210,7 +10269,9 @@
       <c r="C59" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D59" s="3"/>
+      <c r="D59" s="16">
+        <v>1E-3</v>
+      </c>
       <c r="E59" s="7" t="s">
         <v>196</v>
       </c>
@@ -10365,7 +10426,9 @@
       <c r="C60" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D60" s="3"/>
+      <c r="D60" s="16">
+        <v>1.1000000000000001E-3</v>
+      </c>
       <c r="E60">
         <v>0.2525</v>
       </c>
@@ -10524,7 +10587,9 @@
       <c r="C61" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D61" s="3"/>
+      <c r="D61" s="16">
+        <v>2.5000000000000001E-4</v>
+      </c>
       <c r="E61">
         <v>0.2525</v>
       </c>
@@ -10683,7 +10748,9 @@
       <c r="C62" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D62" s="3"/>
+      <c r="D62" s="16">
+        <v>5.2999999999999998E-4</v>
+      </c>
       <c r="E62">
         <v>1.15E-2</v>
       </c>
@@ -10842,7 +10909,9 @@
       <c r="C63" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="D63" s="3"/>
+      <c r="D63" s="16">
+        <v>7.2000000000000005E-4</v>
+      </c>
       <c r="E63">
         <v>3.3999999999999998E-3</v>
       </c>
@@ -11001,7 +11070,9 @@
       <c r="C64" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="D64" s="7"/>
+      <c r="D64" s="7">
+        <v>6.4000000000000005E-4</v>
+      </c>
       <c r="E64" s="2">
         <v>0</v>
       </c>
@@ -11148,7 +11219,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>196</v>
       </c>
@@ -11158,7 +11229,9 @@
       <c r="C65" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="D65" s="7"/>
+      <c r="D65" s="7">
+        <v>6.4000000000000005E-4</v>
+      </c>
       <c r="E65" s="2">
         <v>0</v>
       </c>
@@ -11305,7 +11378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>196</v>
       </c>
@@ -11315,7 +11388,9 @@
       <c r="C66" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="D66" s="14"/>
+      <c r="D66" s="14">
+        <v>5.9999999999999995E-4</v>
+      </c>
       <c r="E66" s="2">
         <v>0</v>
       </c>
@@ -11462,7 +11537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>196</v>
       </c>
@@ -11472,7 +11547,9 @@
       <c r="C67" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="D67" s="7"/>
+      <c r="D67" s="7">
+        <v>5.9999999999999995E-4</v>
+      </c>
       <c r="E67" s="2">
         <v>6.3E-3</v>
       </c>
@@ -11619,7 +11696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:65" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
         <v>196</v>
       </c>
@@ -11629,7 +11706,9 @@
       <c r="C68" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="D68" s="7"/>
+      <c r="D68" s="7">
+        <v>6.9999999999999999E-4</v>
+      </c>
       <c r="E68" s="2">
         <v>0</v>
       </c>
@@ -11776,8 +11855,161 @@
         <v>1</v>
       </c>
     </row>
+    <row r="69" spans="1:65" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="6">
+        <v>4811</v>
+      </c>
+      <c r="D69">
+        <v>9.3999999999999994E-5</v>
+      </c>
+      <c r="J69" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="K69" s="21">
+        <v>14</v>
+      </c>
+      <c r="L69" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="M69" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="N69" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="O69" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="P69" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q69" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="R69" s="21">
+        <v>52</v>
+      </c>
+      <c r="S69" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="T69" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="U69" s="21">
+        <v>22</v>
+      </c>
+      <c r="V69" s="21">
+        <v>9</v>
+      </c>
+      <c r="W69" s="21">
+        <v>7</v>
+      </c>
+      <c r="X69" s="21">
+        <v>1</v>
+      </c>
+      <c r="Y69" s="21">
+        <v>5</v>
+      </c>
+      <c r="Z69" s="21">
+        <v>0</v>
+      </c>
+      <c r="AA69" s="21">
+        <v>16</v>
+      </c>
+      <c r="AB69" s="21">
+        <v>3</v>
+      </c>
+      <c r="AC69" s="21">
+        <v>3</v>
+      </c>
+      <c r="AD69" s="21">
+        <v>1</v>
+      </c>
+      <c r="AE69" s="21">
+        <v>7</v>
+      </c>
+      <c r="AF69" s="21">
+        <v>2</v>
+      </c>
+      <c r="AG69" s="21">
+        <v>6</v>
+      </c>
+      <c r="AH69" s="21">
+        <v>2</v>
+      </c>
+      <c r="AI69" s="21">
+        <v>3</v>
+      </c>
+      <c r="AJ69" s="21">
+        <v>7</v>
+      </c>
+      <c r="AK69" s="21">
+        <v>4</v>
+      </c>
+      <c r="AL69" s="21">
+        <v>3</v>
+      </c>
+      <c r="AM69" s="21">
+        <v>0</v>
+      </c>
+      <c r="AN69" s="21">
+        <v>0</v>
+      </c>
+      <c r="AO69" s="21">
+        <v>0</v>
+      </c>
+      <c r="AP69" s="21">
+        <v>0</v>
+      </c>
+      <c r="AQ69" s="21">
+        <v>0</v>
+      </c>
+      <c r="AR69" s="21">
+        <v>0</v>
+      </c>
+      <c r="AS69" s="21">
+        <v>0</v>
+      </c>
+      <c r="AT69" s="21">
+        <v>0</v>
+      </c>
+      <c r="AU69" s="21">
+        <v>0</v>
+      </c>
+      <c r="AV69" s="21">
+        <v>0</v>
+      </c>
+      <c r="AW69" s="21">
+        <v>0</v>
+      </c>
+      <c r="AX69" s="21">
+        <v>1</v>
+      </c>
+      <c r="AY69" s="21">
+        <v>1</v>
+      </c>
+      <c r="AZ69" s="21">
+        <v>1</v>
+      </c>
+      <c r="BA69" s="21">
+        <v>2</v>
+      </c>
+      <c r="BB69" s="21"/>
+      <c r="BC69" s="21"/>
+      <c r="BD69" s="21"/>
+      <c r="BE69" s="21"/>
+      <c r="BF69" s="21"/>
+      <c r="BG69" s="21"/>
+      <c r="BH69" s="21"/>
+      <c r="BI69" s="21"/>
+      <c r="BJ69" s="21"/>
+      <c r="BK69" s="21"/>
+      <c r="BL69" s="21"/>
+      <c r="BM69" s="21"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11785,8 +12017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:V161"/>
   <sheetViews>
-    <sheetView topLeftCell="E31" workbookViewId="0">
-      <selection activeCell="O39" sqref="O39"/>
+    <sheetView topLeftCell="J46" workbookViewId="0">
+      <selection activeCell="O75" sqref="O75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12132,10 +12364,10 @@
       <c r="I18" s="13"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
-      <c r="N18" s="19">
+      <c r="N18" s="18">
         <v>369</v>
       </c>
-      <c r="O18" s="16">
+      <c r="O18" s="15">
         <v>7.2999999999999996E-4</v>
       </c>
       <c r="P18" s="19"/>
@@ -12615,10 +12847,10 @@
       <c r="I39" s="13"/>
       <c r="J39" s="13"/>
       <c r="K39" s="13"/>
-      <c r="N39" s="19">
+      <c r="N39" s="18">
         <v>571</v>
       </c>
-      <c r="O39" s="16">
+      <c r="O39" s="15">
         <v>7.9000000000000001E-4</v>
       </c>
       <c r="P39" s="19"/>
@@ -12638,10 +12870,10 @@
       <c r="I40" s="13"/>
       <c r="J40" s="13"/>
       <c r="K40" s="13"/>
-      <c r="N40" s="19">
+      <c r="N40" s="18">
         <v>578</v>
       </c>
-      <c r="O40" s="16">
+      <c r="O40" s="15">
         <v>6.3000000000000003E-4</v>
       </c>
       <c r="P40" s="19"/>
@@ -12661,10 +12893,10 @@
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
       <c r="K41" s="13"/>
-      <c r="N41" s="19">
+      <c r="N41" s="18">
         <v>582</v>
       </c>
-      <c r="O41" s="16">
+      <c r="O41" s="15">
         <v>7.1000000000000002E-4</v>
       </c>
       <c r="P41" s="19"/>
@@ -12684,10 +12916,10 @@
       <c r="I42" s="13"/>
       <c r="J42" s="13"/>
       <c r="K42" s="13"/>
-      <c r="N42" s="19">
+      <c r="N42" s="18">
         <v>584</v>
       </c>
-      <c r="O42" s="16">
+      <c r="O42" s="15">
         <v>7.6999999999999996E-4</v>
       </c>
       <c r="P42" s="19"/>
@@ -12707,10 +12939,10 @@
       <c r="I43" s="13"/>
       <c r="J43" s="13"/>
       <c r="K43" s="13"/>
-      <c r="N43" s="19">
+      <c r="N43" s="18">
         <v>589</v>
       </c>
-      <c r="O43" s="16">
+      <c r="O43" s="15">
         <v>8.5999999999999998E-4</v>
       </c>
       <c r="P43" s="19"/>
@@ -12730,10 +12962,10 @@
       <c r="I44" s="13"/>
       <c r="J44" s="13"/>
       <c r="K44" s="13"/>
-      <c r="N44" s="19">
+      <c r="N44" s="18">
         <v>593</v>
       </c>
-      <c r="O44" s="16">
+      <c r="O44" s="15">
         <v>4.6000000000000001E-4</v>
       </c>
       <c r="P44" s="19"/>
@@ -12753,10 +12985,10 @@
       <c r="I45" s="13"/>
       <c r="J45" s="13"/>
       <c r="K45" s="13"/>
-      <c r="N45" s="19">
+      <c r="N45" s="18">
         <v>601</v>
       </c>
-      <c r="O45" s="16">
+      <c r="O45" s="15">
         <v>8.0999999999999996E-4</v>
       </c>
       <c r="P45" s="19"/>
@@ -12776,10 +13008,10 @@
       <c r="I46" s="13"/>
       <c r="J46" s="13"/>
       <c r="K46" s="13"/>
-      <c r="N46" s="19">
+      <c r="N46" s="18">
         <v>606</v>
       </c>
-      <c r="O46" s="16">
+      <c r="O46" s="15">
         <v>8.8999999999999995E-4</v>
       </c>
       <c r="P46" s="19"/>
@@ -12799,10 +13031,10 @@
       <c r="I47" s="13"/>
       <c r="J47" s="13"/>
       <c r="K47" s="13"/>
-      <c r="N47" s="19">
+      <c r="N47" s="18">
         <v>609</v>
       </c>
-      <c r="O47" s="16">
+      <c r="O47" s="15">
         <v>2.1000000000000001E-4</v>
       </c>
       <c r="P47" s="19"/>
@@ -12822,10 +13054,10 @@
       <c r="I48" s="13"/>
       <c r="J48" s="13"/>
       <c r="K48" s="13"/>
-      <c r="N48" s="19">
+      <c r="N48" s="18">
         <v>611</v>
       </c>
-      <c r="O48" s="16">
+      <c r="O48" s="15">
         <v>4.8000000000000001E-4</v>
       </c>
       <c r="P48" s="19"/>
@@ -12845,10 +13077,10 @@
       <c r="I49" s="13"/>
       <c r="J49" s="13"/>
       <c r="K49" s="13"/>
-      <c r="N49" s="19">
+      <c r="N49" s="18">
         <v>619</v>
       </c>
-      <c r="O49" s="16">
+      <c r="O49" s="15">
         <v>7.2999999999999996E-4</v>
       </c>
       <c r="P49" s="19"/>
@@ -12868,10 +13100,10 @@
       <c r="I50" s="13"/>
       <c r="J50" s="13"/>
       <c r="K50" s="13"/>
-      <c r="N50" s="19">
+      <c r="N50" s="18">
         <v>621</v>
       </c>
-      <c r="O50" s="16">
+      <c r="O50" s="15">
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="P50" s="19"/>
@@ -12891,10 +13123,10 @@
       <c r="I51" s="13"/>
       <c r="J51" s="13"/>
       <c r="K51" s="13"/>
-      <c r="N51" s="19">
+      <c r="N51" s="18">
         <v>624</v>
       </c>
-      <c r="O51" s="16">
+      <c r="O51" s="15">
         <v>1E-3</v>
       </c>
       <c r="P51" s="19"/>
@@ -12914,10 +13146,10 @@
       <c r="I52" s="13"/>
       <c r="J52" s="13"/>
       <c r="K52" s="13"/>
-      <c r="N52" s="19">
+      <c r="N52" s="18">
         <v>628</v>
       </c>
-      <c r="O52" s="16">
+      <c r="O52" s="15">
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="P52" s="19"/>
@@ -12937,10 +13169,10 @@
       <c r="I53" s="13"/>
       <c r="J53" s="13"/>
       <c r="K53" s="13"/>
-      <c r="N53" s="19">
+      <c r="N53" s="18">
         <v>667</v>
       </c>
-      <c r="O53" s="16">
+      <c r="O53" s="15">
         <v>1.4E-3</v>
       </c>
       <c r="P53" s="19"/>
@@ -12960,10 +13192,10 @@
       <c r="I54" s="13"/>
       <c r="J54" s="13"/>
       <c r="K54" s="13"/>
-      <c r="N54" s="19">
+      <c r="N54" s="18">
         <v>673</v>
       </c>
-      <c r="O54" s="16">
+      <c r="O54" s="15">
         <v>3.8000000000000002E-4</v>
       </c>
       <c r="P54" s="19"/>
@@ -12983,10 +13215,10 @@
       <c r="I55" s="13"/>
       <c r="J55" s="13"/>
       <c r="K55" s="13"/>
-      <c r="N55" s="19">
+      <c r="N55" s="18">
         <v>678</v>
       </c>
-      <c r="O55" s="16">
+      <c r="O55" s="15">
         <v>5.2999999999999998E-4</v>
       </c>
       <c r="P55" s="19"/>
@@ -13006,10 +13238,10 @@
       <c r="I56" s="13"/>
       <c r="J56" s="13"/>
       <c r="K56" s="13"/>
-      <c r="N56" s="19">
+      <c r="N56" s="18">
         <v>682</v>
       </c>
-      <c r="O56" s="16">
+      <c r="O56" s="15">
         <v>7.2000000000000005E-4</v>
       </c>
       <c r="P56" s="19"/>
@@ -13029,10 +13261,10 @@
       <c r="I57" s="13"/>
       <c r="J57" s="13"/>
       <c r="K57" s="13"/>
-      <c r="N57" s="19">
+      <c r="N57" s="18">
         <v>692</v>
       </c>
-      <c r="O57" s="16">
+      <c r="O57" s="15">
         <v>2.3999999999999998E-3</v>
       </c>
       <c r="P57" s="19"/>
@@ -13052,10 +13284,10 @@
       <c r="I58" s="13"/>
       <c r="J58" s="13"/>
       <c r="K58" s="13"/>
-      <c r="N58" s="19">
+      <c r="N58" s="18">
         <v>694</v>
       </c>
-      <c r="O58" s="16">
+      <c r="O58" s="15">
         <v>5.6999999999999998E-4</v>
       </c>
       <c r="P58" s="19"/>
@@ -13075,10 +13307,10 @@
       <c r="I59" s="13"/>
       <c r="J59" s="13"/>
       <c r="K59" s="13"/>
-      <c r="N59" s="19">
+      <c r="N59" s="18">
         <v>701</v>
       </c>
-      <c r="O59" s="16">
+      <c r="O59" s="15">
         <v>6.6E-4</v>
       </c>
       <c r="P59" s="19"/>
@@ -13098,10 +13330,10 @@
       <c r="I60" s="13"/>
       <c r="J60" s="13"/>
       <c r="K60" s="13"/>
-      <c r="N60" s="19">
+      <c r="N60" s="18">
         <v>706</v>
       </c>
-      <c r="O60" s="16">
+      <c r="O60" s="15">
         <v>5.6999999999999998E-4</v>
       </c>
       <c r="P60" s="19"/>
@@ -13121,10 +13353,10 @@
       <c r="I61" s="13"/>
       <c r="J61" s="13"/>
       <c r="K61" s="13"/>
-      <c r="N61" s="19">
+      <c r="N61" s="18">
         <v>707</v>
       </c>
-      <c r="O61" s="16">
+      <c r="O61" s="15">
         <v>4.4999999999999999E-4</v>
       </c>
       <c r="P61" s="19"/>
@@ -13167,10 +13399,10 @@
       <c r="I63" s="13"/>
       <c r="J63" s="13"/>
       <c r="K63" s="13"/>
-      <c r="N63" s="19">
+      <c r="N63" s="18">
         <v>730</v>
       </c>
-      <c r="O63" s="16">
+      <c r="O63" s="15">
         <v>5.8E-4</v>
       </c>
       <c r="P63" s="19"/>

</xml_diff>